<commit_message>
LMDI: Fikset tillatt adressetype 8375d563b47ec2b0876856ebe3f7969f60c0ad74
</commit_message>
<xml_diff>
--- a/currentbuild/StructureDefinition-lmdi-patient.xlsx
+++ b/currentbuild/StructureDefinition-lmdi-patient.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4746" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4745" uniqueCount="718">
   <si>
     <t>Property</t>
   </si>
@@ -1544,22 +1544,23 @@
     <t>Patient.address.type</t>
   </si>
   <si>
+    <t>postal | physical | both</t>
+  </si>
+  <si>
+    <t>Distinguishes between physical addresses (those you can visit) and mailing addresses (e.g. PO Boxes and care-of addresses). Most addresses are both.
+Mapping of values to other Norwegian CodeSystems is documented in the implementation guide. In general the address used for visiting the person should have use "home" and type "physical" or "both". The "official" flag can be either true or false.</t>
+  </si>
+  <si>
+    <t>The definition of Address states that "address is intended to describe postal addresses, not physical locations". However, many applications track whether an address has a dual purpose of being a location that can be visited as well as being a valid delivery destination, and Postal addresses are often used as proxies for physical locations (also see the [Location](http://hl7.org/fhir/R4/location.html#) resource).</t>
+  </si>
+  <si>
     <t>physical</t>
   </si>
   <si>
-    <t>Adressetypen er begrenset til physical (fysisk adresse)</t>
-  </si>
-  <si>
-    <t>The definition of Address states that "address is intended to describe postal addresses, not physical locations". However, many applications track whether an address has a dual purpose of being a location that can be visited as well as being a valid delivery destination, and Postal addresses are often used as proxies for physical locations (also see the [Location](http://hl7.org/fhir/R4/location.html#) resource).</t>
-  </si>
-  <si>
     <t>both</t>
   </si>
   <si>
-    <t>The type of an address (physical / postal).</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/address-type|4.0.1</t>
+    <t>http://hl7.no/fhir/ig/lmdi/ValueSet/lmdi-address-type</t>
   </si>
   <si>
     <t>Address.type</t>
@@ -12752,10 +12753,10 @@
         <v>81</v>
       </c>
       <c r="S87" t="s" s="2">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="T87" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="U87" t="s" s="2">
         <v>81</v>
@@ -12769,9 +12770,7 @@
       <c r="X87" t="s" s="2">
         <v>224</v>
       </c>
-      <c r="Y87" t="s" s="2">
-        <v>497</v>
-      </c>
+      <c r="Y87" s="2"/>
       <c r="Z87" t="s" s="2">
         <v>498</v>
       </c>

</xml_diff>